<commit_message>
Auto bat commit friday
</commit_message>
<xml_diff>
--- a/src/test/resources/Userdata.xlsx
+++ b/src/test/resources/Userdata.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E\workspaces\workSpace_RestAssured_P1\PetStoreApiAutomation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCCAB76-4735-440A-A20E-98B3A319DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF0D2628-A76B-48EE-8E71-87E5FD99D157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" r:id="rId1"/>
+    <sheet name="booking" sheetId="2" r:id="rId2"/>
+    <sheet name="booking_data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>UserID</t>
   </si>
@@ -115,6 +117,51 @@
   </si>
   <si>
     <t>LLhghfjhfj88</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>password123</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>totalprice</t>
+  </si>
+  <si>
+    <t>depositpaid</t>
+  </si>
+  <si>
+    <t>additionalneeds</t>
+  </si>
+  <si>
+    <t>checkin</t>
+  </si>
+  <si>
+    <t>checkout</t>
+  </si>
+  <si>
+    <t>Akram</t>
+  </si>
+  <si>
+    <t>Wasim</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>JungleTour-</t>
   </si>
 </sst>
 </file>
@@ -188,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -197,6 +244,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -482,7 +535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -696,4 +749,107 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021EB4BE-423F-4752-BAB3-DD773355A032}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9911A16-E897-497B-A45F-E5347FC72DC8}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44927</v>
+      </c>
+      <c r="F2" s="4">
+        <v>44928</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>